<commit_message>
DEV: Update Price Analysis xlsx
</commit_message>
<xml_diff>
--- a/DataAnalysis/Data/output/price_analysis.xlsx
+++ b/DataAnalysis/Data/output/price_analysis.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="district_price_per_m2_extremes" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="district_adjusted_price_per_m2_extremes" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="price_comparison" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,55 +436,110 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>district</t>
+          <t>District</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>min</t>
+          <t>Price_SharedFlats</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>max</t>
+          <t>Price_Adjusted_SharedFlats</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Price_HousingMarket</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Diff_SharedFlats_vs_HousingMarket</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Diff_SharedFlats_Adjusted_vs_HousingMarket</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Diff_Original_%</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Diff_Adjusted_%</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mitte</t>
+          <t>Spandau</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3.5</v>
+        <v>30.54086538461539</v>
       </c>
       <c r="D2" t="n">
-        <v>90</v>
+        <v>20.39186391789341</v>
+      </c>
+      <c r="E2" t="n">
+        <v>9.341384152837394</v>
+      </c>
+      <c r="F2" t="n">
+        <v>21.19948123177799</v>
+      </c>
+      <c r="G2" t="n">
+        <v>11.05047976505602</v>
+      </c>
+      <c r="H2" t="n">
+        <v>226.9415419056369</v>
+      </c>
+      <c r="I2" t="n">
+        <v>118.2959568331155</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Friedrichshain-Kreuzberg</t>
+          <t>Reinickendorf</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3.75</v>
+        <v>30</v>
       </c>
       <c r="D3" t="n">
-        <v>85</v>
+        <v>20.76984441268803</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10.47216271058341</v>
+      </c>
+      <c r="F3" t="n">
+        <v>19.5278372894166</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10.29768170210462</v>
+      </c>
+      <c r="H3" t="n">
+        <v>186.4737765168728</v>
+      </c>
+      <c r="I3" t="n">
+        <v>98.33385888568699</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -493,42 +547,87 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3.809523809523809</v>
+        <v>30</v>
       </c>
       <c r="D4" t="n">
-        <v>100</v>
+        <v>18.53202099840722</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11.1179280113382</v>
+      </c>
+      <c r="F4" t="n">
+        <v>18.8820719886618</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.414092987069013</v>
+      </c>
+      <c r="H4" t="n">
+        <v>169.8344508923392</v>
+      </c>
+      <c r="I4" t="n">
+        <v>66.68592366768365</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Neukölln</t>
+          <t>Marzahn-Hellersdorf</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3.846153846153846</v>
+        <v>30</v>
       </c>
       <c r="D5" t="n">
-        <v>76.92307692307692</v>
+        <v>17.19230769230769</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10.3678218974249</v>
+      </c>
+      <c r="F5" t="n">
+        <v>19.6321781025751</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6.824485794882793</v>
+      </c>
+      <c r="H5" t="n">
+        <v>189.3568224532409</v>
+      </c>
+      <c r="I5" t="n">
+        <v>65.82371748281884</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pankow</t>
+          <t>Tempelhof-Schöneberg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4.444444444444445</v>
+        <v>29.11538461538461</v>
       </c>
       <c r="D6" t="n">
-        <v>89</v>
+        <v>18.47527263222872</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12.13993599794491</v>
+      </c>
+      <c r="F6" t="n">
+        <v>16.9754486174397</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6.335336634283806</v>
+      </c>
+      <c r="H6" t="n">
+        <v>139.8314506790923</v>
+      </c>
+      <c r="I6" t="n">
+        <v>52.18591461566414</v>
       </c>
     </row>
     <row r="7">
@@ -537,338 +636,215 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Treptow-Köpenick</t>
+          <t>Neukölln</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>27.5</v>
       </c>
       <c r="D7" t="n">
-        <v>74.2</v>
+        <v>17.46796253072736</v>
+      </c>
+      <c r="E7" t="n">
+        <v>11.52667883982897</v>
+      </c>
+      <c r="F7" t="n">
+        <v>15.97332116017103</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5.941283690898384</v>
+      </c>
+      <c r="H7" t="n">
+        <v>138.5769603034072</v>
+      </c>
+      <c r="I7" t="n">
+        <v>51.5437601190816</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tempelhof-Schöneberg</t>
+          <t>Steglitz-Zehlendorf</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>63.33333333333334</v>
+        <v>19.41263242590854</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.23848794563714</v>
+      </c>
+      <c r="F8" t="n">
+        <v>16.76151205436286</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6.174144480271407</v>
+      </c>
+      <c r="H8" t="n">
+        <v>126.6119826009795</v>
+      </c>
+      <c r="I8" t="n">
+        <v>46.63783738463992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Charlottenburg-Wilmersdorf</t>
+          <t>Pankow</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6.666666666666667</v>
+        <v>29.66666666666667</v>
       </c>
       <c r="D9" t="n">
-        <v>105</v>
+        <v>18.87490810992743</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13.63586323304723</v>
+      </c>
+      <c r="F9" t="n">
+        <v>16.03080343361944</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5.2390448768802</v>
+      </c>
+      <c r="H9" t="n">
+        <v>117.5635393201066</v>
+      </c>
+      <c r="I9" t="n">
+        <v>38.42107233946949</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Steglitz-Zehlendorf</t>
+          <t>Treptow-Köpenick</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6.818181818181818</v>
+        <v>29.32183908045977</v>
       </c>
       <c r="D10" t="n">
-        <v>57</v>
+        <v>17.33324252455699</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13.02911475531228</v>
+      </c>
+      <c r="F10" t="n">
+        <v>16.29272432514748</v>
+      </c>
+      <c r="G10" t="n">
+        <v>4.304127769244703</v>
+      </c>
+      <c r="H10" t="n">
+        <v>125.0485902620863</v>
+      </c>
+      <c r="I10" t="n">
+        <v>33.03469076814913</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Reinickendorf</t>
+          <t>Charlottenburg-Wilmersdorf</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.666666666666667</v>
+        <v>28.84615384615385</v>
       </c>
       <c r="D11" t="n">
-        <v>70</v>
+        <v>19.28929627733574</v>
+      </c>
+      <c r="E11" t="n">
+        <v>16.42457502011024</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12.4215788260436</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.864721257225501</v>
+      </c>
+      <c r="H11" t="n">
+        <v>75.62800748777138</v>
+      </c>
+      <c r="I11" t="n">
+        <v>17.44167659569844</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Marzahn-Hellersdorf</t>
+          <t>Mitte</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10.525</v>
+        <v>29.33333333333333</v>
       </c>
       <c r="D12" t="n">
-        <v>57.91666666666666</v>
+        <v>17.97484666745213</v>
+      </c>
+      <c r="E12" t="n">
+        <v>17.57533810105219</v>
+      </c>
+      <c r="F12" t="n">
+        <v>11.75799523228114</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.3995085663999376</v>
+      </c>
+      <c r="H12" t="n">
+        <v>66.90053508317557</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2.273120233038476</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Spandau</t>
+          <t>Friedrichshain-Kreuzberg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>12.33333333333333</v>
+        <v>28.125</v>
       </c>
       <c r="D13" t="n">
-        <v>63.63636363636363</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>district</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>min</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>max</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Treptow-Köpenick</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2.243068108490236</v>
-      </c>
-      <c r="D2" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Steglitz-Zehlendorf</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2.279234990546991</v>
-      </c>
-      <c r="D3" t="n">
-        <v>50.52631578947368</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Mitte</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2.396483744492055</v>
-      </c>
-      <c r="D4" t="n">
-        <v>56.25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Pankow</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3.170910683971305</v>
-      </c>
-      <c r="D5" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Friedrichshain-Kreuzberg</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>3.329262599152275</v>
-      </c>
-      <c r="D6" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Lichtenberg</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>3.823818594317278</v>
-      </c>
-      <c r="D7" t="n">
-        <v>63.5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Neukölln</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>3.992189913074174</v>
-      </c>
-      <c r="D8" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Tempelhof-Schöneberg</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>4.931506849315069</v>
-      </c>
-      <c r="D9" t="n">
-        <v>63.33333333333334</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Charlottenburg-Wilmersdorf</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>5.253016420212283</v>
-      </c>
-      <c r="D10" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Marzahn-Hellersdorf</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>5.866666666666666</v>
-      </c>
-      <c r="D11" t="n">
-        <v>34.75</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Reinickendorf</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>6.040968883244126</v>
-      </c>
-      <c r="D12" t="n">
-        <v>46.85661571327998</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Spandau</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>8.962293824373734</v>
-      </c>
-      <c r="D13" t="n">
-        <v>48.27022791310292</v>
+        <v>16.67864346704081</v>
+      </c>
+      <c r="E13" t="n">
+        <v>16.43813941562651</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11.68686058437349</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.2405040514142982</v>
+      </c>
+      <c r="H13" t="n">
+        <v>71.09600599483703</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.463085604357808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>